<commit_message>
add shift line, Edit export excel, edit load data sevire borek
</commit_message>
<xml_diff>
--- a/LineStatusClient/Common/template.xlsx
+++ b/LineStatusClient/Common/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latitude 5520\Desktop\LineStatusClient\LineStatusClient\Common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_RTC\09_SVWS.23.002_DichVuHoTroLapTrinhChoNhaMay\02_LineStatus\source code\CLIENT\line-status-client\LineStatusClient\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5C20B1-58B5-47F1-AA9A-AB29488C20B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E71BD-B2F9-4676-AD33-DC0EB2A72FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8156288-2D40-4FA0-B048-C806DF17F777}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8156288-2D40-4FA0-B048-C806DF17F777}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Trạng Thái</t>
   </si>
@@ -41,12 +41,21 @@
   <si>
     <t>Bảng quản lý sản xuất dây chuyền Line-placeholder ngày:  datetime</t>
   </si>
+  <si>
+    <t>Tổng thời gian hoạt động</t>
+  </si>
+  <si>
+    <t>Chạy</t>
+  </si>
+  <si>
+    <t>Dừng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,16 +70,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,14 +113,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,9 +203,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +243,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -287,7 +349,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,50 +499,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392BAA5B-3586-4600-A9B0-AADA1B8C4FAA}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="7" width="10.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.36251157407407408</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.36736111111111108</v>
       </c>
@@ -488,7 +566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.36745370370370373</v>
       </c>
@@ -496,7 +574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.36954861111111109</v>
       </c>
@@ -504,7 +582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.37234953703703705</v>
       </c>
@@ -512,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.3746990740740741</v>
       </c>
@@ -520,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.38009259259259259</v>
       </c>
@@ -528,7 +606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.38260416666666663</v>
       </c>
@@ -536,7 +614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.3870601851851852</v>
       </c>

</xml_diff>